<commit_message>
Conference scheduling: Fix XLS test
Signed-off-by: Lukáš Petrovický <lukas@petrovicky.net>
</commit_message>
<xml_diff>
--- a/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/drools/testConferenceSchedulingConstraints.xlsx
+++ b/optaplanner-examples/src/test/resources/org/optaplanner/examples/conferencescheduling/optional/score/drools/testConferenceSchedulingConstraints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="56"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,10 +30,10 @@
     <sheet name="Talk prerequisite talks 4" sheetId="20" state="visible" r:id="rId21"/>
     <sheet name="Talk prerequisite talks 5" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Talk prerequisite talks 6" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="Talk mutually-exclusive-talks tags 1" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="Talk mutually-exclusive-talks tags 2" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="Talk mutually-exclusive-talks tags 3" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="Talk mutually-exclusive-talks tags 4" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Talk mutually-exclusive-talks t" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Talk mutually-exclusive-talks-1" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Talk mutually-exclusive-talks-2" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Talk mutually-exclusive-talks-3" sheetId="26" state="visible" r:id="rId27"/>
     <sheet name="Consecutive talks pause 1" sheetId="27" state="visible" r:id="rId28"/>
     <sheet name="Consecutive talks pause 2" sheetId="28" state="visible" r:id="rId29"/>
     <sheet name="Consecutive talks pause 3" sheetId="29" state="visible" r:id="rId30"/>
@@ -582,7 +582,7 @@
     <t xml:space="preserve">Constraint package</t>
   </si>
   <si>
-    <t xml:space="preserve">org.optaplanner.examples.conferencescheduling.solver</t>
+    <t xml:space="preserve">org.optaplanner.examples.conferencescheduling.score</t>
   </si>
   <si>
     <t xml:space="preserve">Constraint name</t>
@@ -735,7 +735,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;PRAVDA&quot;;&quot;PRAVDA&quot;;&quot;NEPRAVDA&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -898,12 +898,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -969,26 +969,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="C27" activeCellId="1" sqref="B1 C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="141.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1432,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1442,27 +1441,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1642,7 +1641,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1651,27 +1650,27 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1834,7 +1833,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1843,27 +1842,27 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2027,7 +2026,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2036,27 +2035,27 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2219,7 +2218,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2228,27 +2227,27 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2411,7 +2410,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2420,27 +2419,27 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2606,7 +2605,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2615,27 +2614,27 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2815,7 +2814,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2824,27 +2823,27 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3026,7 +3025,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3035,27 +3034,27 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3239,7 +3238,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3248,29 +3247,29 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3440,7 +3439,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3449,7 +3448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3460,16 +3459,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D18" activeCellId="1" sqref="B1 D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,7 +3591,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3602,27 +3600,27 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3788,7 +3786,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3797,27 +3795,27 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3983,7 +3981,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3992,27 +3990,27 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4180,7 +4178,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4189,27 +4187,27 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4390,7 +4388,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4399,27 +4397,27 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4601,7 +4599,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4610,27 +4608,27 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4814,7 +4812,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4823,27 +4821,27 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5032,7 +5030,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5041,29 +5039,29 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5260,7 +5258,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5269,29 +5267,29 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5471,7 +5469,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5480,29 +5478,29 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5682,7 +5680,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5691,7 +5689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5702,21 +5700,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="E17" activeCellId="1" sqref="B1 E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1015" min="12" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1016" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5871,7 +5868,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5880,29 +5877,29 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6099,7 +6096,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6108,29 +6105,29 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="6" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="28" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6310,7 +6307,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6319,27 +6316,27 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6533,7 +6530,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6542,27 +6539,27 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6756,7 +6753,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6765,27 +6762,27 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6975,7 +6972,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6984,27 +6981,27 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7198,7 +7195,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7207,27 +7204,27 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7425,7 +7422,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7434,27 +7431,27 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7638,7 +7635,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7647,27 +7644,27 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7851,7 +7848,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7860,27 +7857,27 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8064,7 +8061,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8073,7 +8070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8084,12 +8081,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="1" sqref="B1 A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.01"/>
@@ -8101,9 +8098,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="17" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8266,7 +8262,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8275,27 +8271,27 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8479,7 +8475,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8488,27 +8484,27 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8692,7 +8688,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8701,27 +8697,27 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8905,7 +8901,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8914,27 +8910,27 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9120,7 +9116,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9129,27 +9125,27 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9335,7 +9331,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9344,27 +9340,27 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9550,7 +9546,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9559,27 +9555,27 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9765,7 +9761,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9774,27 +9770,27 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9988,7 +9984,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9997,27 +9993,27 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10183,7 +10179,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10192,27 +10188,27 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10382,7 +10378,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10391,7 +10387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -10402,10 +10398,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="1" sqref="B1 A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.95"/>
@@ -10426,13 +10422,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="25" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="31" min="28" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="28" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12515,7 +12510,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12524,27 +12519,27 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12714,7 +12709,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12723,27 +12718,27 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12913,7 +12908,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -12922,27 +12917,27 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13112,7 +13107,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13121,7 +13116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
@@ -13133,15 +13128,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13304,7 +13299,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13313,7 +13308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
@@ -13325,15 +13320,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13515,7 +13510,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13524,7 +13519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
@@ -13536,15 +13531,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13726,7 +13721,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13735,7 +13730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
@@ -13747,15 +13742,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13937,7 +13932,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -13946,27 +13941,27 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G37" activeCellId="0" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14148,7 +14143,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14157,27 +14152,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14341,7 +14336,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14350,27 +14345,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14533,7 +14528,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14542,27 +14537,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14728,7 +14723,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -14737,27 +14732,27 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FF00DCFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="11" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="11" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="11" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14922,7 +14917,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>